<commit_message>
Finished draft of Requirements Specifications.
</commit_message>
<xml_diff>
--- a/Components/Components and Pricing Sheet.xlsx
+++ b/Components/Components and Pricing Sheet.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="32">
   <si>
     <t>Manufacturer</t>
   </si>
@@ -99,6 +99,27 @@
   </si>
   <si>
     <t>4-16 demux</t>
+  </si>
+  <si>
+    <t>Final Build</t>
+  </si>
+  <si>
+    <t>Prototype</t>
+  </si>
+  <si>
+    <t>CD4043BE</t>
+  </si>
+  <si>
+    <t>Quad SR latch</t>
+  </si>
+  <si>
+    <t>Thru-Hole</t>
+  </si>
+  <si>
+    <t>CD4043BDWR</t>
+  </si>
+  <si>
+    <t>SMT</t>
   </si>
 </sst>
 </file>
@@ -132,12 +153,30 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -152,13 +191,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -439,10 +484,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:I96"/>
+  <dimension ref="A2:L96"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -454,7 +499,7 @@
     <col min="5" max="5" width="8.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -483,184 +528,230 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="1">
+      <c r="E3" s="5">
         <v>0.107</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="3">
         <v>3</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="3">
         <f>F3*4</f>
         <v>12</v>
       </c>
-      <c r="H3" s="1">
+      <c r="H3" s="5">
         <f>E3*G3</f>
         <v>1.284</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3" s="3" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="L3" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="1">
+      <c r="E4" s="5">
         <v>0.09</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="3">
         <v>3</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="3">
         <f t="shared" ref="G4:G17" si="0">F4*4</f>
         <v>12</v>
       </c>
-      <c r="H4" s="1">
+      <c r="H4" s="5">
         <f t="shared" ref="H4:H17" si="1">E4*G4</f>
         <v>1.08</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I4" s="3" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="L4" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="1">
+      <c r="E5" s="5">
         <v>0.09</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="3">
         <v>3</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="H5" s="1">
+      <c r="H5" s="5">
         <f t="shared" si="1"/>
         <v>1.08</v>
       </c>
-      <c r="I5" t="s">
+      <c r="I5" s="3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="1">
+      <c r="E6" s="5">
         <v>0.27600000000000002</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="3">
         <v>9</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="3">
         <f t="shared" si="0"/>
         <v>36</v>
       </c>
-      <c r="H6" s="1">
+      <c r="H6" s="5">
         <f t="shared" si="1"/>
         <v>9.9359999999999999</v>
       </c>
-      <c r="I6" t="s">
+      <c r="I6" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E7" s="1">
+      <c r="E7" s="9">
         <v>1.61</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="8">
         <v>1</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="8">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="H7" s="1">
+      <c r="H7" s="9">
         <f t="shared" si="1"/>
         <v>6.44</v>
       </c>
-      <c r="I7" t="s">
+      <c r="I7" s="8" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E8" s="1"/>
-      <c r="G8">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H8" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E9" s="1"/>
-      <c r="G9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H9" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" s="6">
+        <v>0.6</v>
+      </c>
+      <c r="F8" s="4">
+        <v>3</v>
+      </c>
+      <c r="G8" s="4">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="H8" s="6">
+        <f t="shared" si="1"/>
+        <v>7.1999999999999993</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="5">
+        <v>0.67</v>
+      </c>
+      <c r="F9" s="3">
+        <v>3</v>
+      </c>
+      <c r="G9" s="3">
+        <f t="shared" ref="G9" si="2">F9*4</f>
+        <v>12</v>
+      </c>
+      <c r="H9" s="5">
+        <f t="shared" ref="H9" si="3">E9*G9</f>
+        <v>8.0400000000000009</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E10" s="1"/>
       <c r="G10">
         <f t="shared" si="0"/>
@@ -671,7 +762,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E11" s="1"/>
       <c r="G11">
         <f t="shared" si="0"/>
@@ -682,7 +773,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E12" s="1"/>
       <c r="G12">
         <f t="shared" si="0"/>
@@ -693,7 +784,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E13" s="1"/>
       <c r="G13">
         <f t="shared" si="0"/>
@@ -704,7 +795,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E14" s="1"/>
       <c r="G14">
         <f t="shared" si="0"/>
@@ -715,7 +806,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E15" s="1"/>
       <c r="G15">
         <f t="shared" si="0"/>
@@ -726,7 +817,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E16" s="1"/>
       <c r="G16">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
New datasheets and updated components spreadsheet with new components and prototype parts order.
</commit_message>
<xml_diff>
--- a/Components/Components and Pricing Sheet.xlsx
+++ b/Components/Components and Pricing Sheet.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="46">
   <si>
     <t>Manufacturer</t>
   </si>
@@ -41,9 +41,6 @@
     <t>Price</t>
   </si>
   <si>
-    <t>Notes</t>
-  </si>
-  <si>
     <t>Lite-On</t>
   </si>
   <si>
@@ -53,18 +50,12 @@
     <t>LTL1CHKEKNN</t>
   </si>
   <si>
-    <t>LTL1CHKFKNN</t>
-  </si>
-  <si>
     <t>Red LED</t>
   </si>
   <si>
     <t>Green LED</t>
   </si>
   <si>
-    <t>Orange LED</t>
-  </si>
-  <si>
     <t>Mouser</t>
   </si>
   <si>
@@ -80,12 +71,6 @@
     <t>Fairchild</t>
   </si>
   <si>
-    <t>2n7002/NDS7002A</t>
-  </si>
-  <si>
-    <t>n-channel FET</t>
-  </si>
-  <si>
     <t>3mm</t>
   </si>
   <si>
@@ -120,6 +105,63 @@
   </si>
   <si>
     <t>SMT</t>
+  </si>
+  <si>
+    <t>NXP Semiconductor</t>
+  </si>
+  <si>
+    <t>HEF4067BT</t>
+  </si>
+  <si>
+    <t>HEF4067BPN</t>
+  </si>
+  <si>
+    <t>LTL1CHKSKNN</t>
+  </si>
+  <si>
+    <t>Yellow LED</t>
+  </si>
+  <si>
+    <t>2n7002DW</t>
+  </si>
+  <si>
+    <t>Dual N-channel FET</t>
+  </si>
+  <si>
+    <t>N-Channel FET</t>
+  </si>
+  <si>
+    <t>Prototype Order 10/26</t>
+  </si>
+  <si>
+    <t>Qty</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>2n7000</t>
+  </si>
+  <si>
+    <t>Ordered</t>
+  </si>
+  <si>
+    <t>Substituted</t>
+  </si>
+  <si>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>Final</t>
+  </si>
+  <si>
+    <t>n/a</t>
+  </si>
+  <si>
+    <t>final</t>
+  </si>
+  <si>
+    <t>Shipping</t>
   </si>
 </sst>
 </file>
@@ -153,7 +195,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -174,7 +216,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -191,19 +245,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -484,10 +542,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:L96"/>
+  <dimension ref="A2:U97"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="Q19" sqref="Q19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -497,9 +555,13 @@
     <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.28515625" customWidth="1"/>
+    <col min="12" max="12" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="21" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="18.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -516,275 +578,555 @@
         <v>4</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="O2" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="P2" s="8"/>
+      <c r="Q2" s="8"/>
+      <c r="R2" s="8"/>
+      <c r="S2" s="8"/>
+      <c r="T2" s="8"/>
+      <c r="U2" s="8"/>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="B3" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="5">
+      <c r="C3" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="7">
         <v>0.107</v>
       </c>
-      <c r="F3" s="3">
+      <c r="F3" s="6">
         <v>3</v>
       </c>
-      <c r="G3" s="3">
+      <c r="G3" s="6">
         <f>F3*4</f>
         <v>12</v>
       </c>
-      <c r="H3" s="5">
+      <c r="H3" s="7">
         <f>E3*G3</f>
         <v>1.284</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="I3" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="L3" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="L3" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="O3" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="P3" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q3" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="R3" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="S3" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="T3" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="U3" s="13" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="7">
+        <v>0.09</v>
+      </c>
+      <c r="F4" s="6">
+        <v>3</v>
+      </c>
+      <c r="G4" s="6">
+        <f t="shared" ref="G4:G18" si="0">F4*4</f>
+        <v>12</v>
+      </c>
+      <c r="H4" s="7">
+        <f t="shared" ref="H4:H18" si="1">E4*G4</f>
+        <v>1.08</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="J4" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="O4" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="P4" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="5">
-        <v>0.09</v>
-      </c>
-      <c r="F4" s="3">
+      <c r="Q4" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="R4" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="S4" s="9">
+        <v>0.107</v>
+      </c>
+      <c r="T4" s="8">
+        <v>12</v>
+      </c>
+      <c r="U4" s="9">
+        <f>S4*T4</f>
+        <v>1.284</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="7">
+        <v>0.10199999999999999</v>
+      </c>
+      <c r="F5" s="6">
         <v>3</v>
       </c>
-      <c r="G4" s="3">
-        <f t="shared" ref="G4:G17" si="0">F4*4</f>
-        <v>12</v>
-      </c>
-      <c r="H4" s="5">
-        <f t="shared" ref="H4:H17" si="1">E4*G4</f>
-        <v>1.08</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L4" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" s="5">
-        <v>0.09</v>
-      </c>
-      <c r="F5" s="3">
-        <v>3</v>
-      </c>
-      <c r="G5" s="3">
+      <c r="G5" s="6">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="H5" s="5">
+      <c r="H5" s="7">
         <f t="shared" si="1"/>
+        <v>1.224</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="J5" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="L5" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="O5" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="P5" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q5" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="R5" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="S5" s="9">
+        <v>0.09</v>
+      </c>
+      <c r="T5" s="8">
+        <v>12</v>
+      </c>
+      <c r="U5" s="9">
+        <f t="shared" ref="U5:U9" si="2">S5*T5</f>
         <v>1.08</v>
       </c>
-      <c r="I5" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E6" s="5">
         <v>0.27600000000000002</v>
       </c>
       <c r="F6" s="3">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="G6" s="3">
         <f t="shared" si="0"/>
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="H6" s="5">
         <f t="shared" si="1"/>
-        <v>9.9359999999999999</v>
+        <v>5.5200000000000005</v>
       </c>
       <c r="I6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="L6" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="O6" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="P6" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q6" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="R6" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="S6" s="9">
+        <v>0.10199999999999999</v>
+      </c>
+      <c r="T6" s="8">
+        <v>12</v>
+      </c>
+      <c r="U6" s="9">
+        <f t="shared" si="2"/>
+        <v>1.224</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="7">
+        <v>0.24</v>
+      </c>
+      <c r="F7" s="6">
+        <v>10</v>
+      </c>
+      <c r="G7" s="6">
+        <v>10</v>
+      </c>
+      <c r="H7" s="7">
+        <f t="shared" ref="H7" si="3">E7*G7</f>
+        <v>2.4</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="J7" s="6" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="E7" s="9">
+      <c r="O7" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="P7" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q7" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="R7" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="S7" s="9">
+        <v>0.24</v>
+      </c>
+      <c r="T7" s="8">
+        <v>10</v>
+      </c>
+      <c r="U7" s="9">
+        <f t="shared" si="2"/>
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A8" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="12">
         <v>1.61</v>
       </c>
-      <c r="F7" s="8">
+      <c r="F8" s="11">
         <v>1</v>
       </c>
-      <c r="G7" s="8">
+      <c r="G8" s="11">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="H7" s="9">
+      <c r="H8" s="12">
         <f t="shared" si="1"/>
         <v>6.44</v>
       </c>
-      <c r="I7" s="8" t="s">
+      <c r="I8" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="J8" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="O8" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="P8" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q8" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="R8" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="S8" s="9">
+        <v>5.43</v>
+      </c>
+      <c r="T8" s="8">
+        <v>1</v>
+      </c>
+      <c r="U8" s="9">
+        <f t="shared" si="2"/>
+        <v>5.43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="7">
+        <v>0.6</v>
+      </c>
+      <c r="F9" s="6">
+        <v>3</v>
+      </c>
+      <c r="G9" s="6">
+        <v>4</v>
+      </c>
+      <c r="H9" s="7">
+        <f t="shared" si="1"/>
+        <v>2.4</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="J9" s="6" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+      <c r="O9" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="P9" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q9" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="R9" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="S9" s="9">
+        <v>0.6</v>
+      </c>
+      <c r="T9" s="8">
+        <v>4</v>
+      </c>
+      <c r="U9" s="9">
+        <f t="shared" si="2"/>
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="5">
+        <v>0.67</v>
+      </c>
+      <c r="F10" s="3">
+        <v>3</v>
+      </c>
+      <c r="G10" s="3">
+        <f t="shared" ref="G10" si="4">F10*4</f>
+        <v>12</v>
+      </c>
+      <c r="H10" s="5">
+        <f t="shared" ref="H10" si="5">E10*G10</f>
+        <v>8.0400000000000009</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="O10" s="8"/>
+      <c r="P10" s="8"/>
+      <c r="Q10" s="8"/>
+      <c r="R10" s="8"/>
+      <c r="S10" s="8"/>
+      <c r="T10" s="8"/>
+      <c r="U10" s="8"/>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="B11" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" s="7">
+        <v>5.43</v>
+      </c>
+      <c r="F11" s="6">
+        <v>1</v>
+      </c>
+      <c r="G11" s="6">
+        <v>1</v>
+      </c>
+      <c r="H11" s="7">
+        <f t="shared" si="1"/>
+        <v>5.43</v>
+      </c>
+      <c r="I11" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="J11" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="O11" s="8"/>
+      <c r="P11" s="8"/>
+      <c r="Q11" s="8"/>
+      <c r="R11" s="8"/>
+      <c r="S11" s="8"/>
+      <c r="T11" s="8"/>
+      <c r="U11" s="8"/>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D8" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E8" s="6">
-        <v>0.6</v>
-      </c>
-      <c r="F8" s="4">
-        <v>3</v>
-      </c>
-      <c r="G8" s="4">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-      <c r="H8" s="6">
-        <f t="shared" si="1"/>
-        <v>7.1999999999999993</v>
-      </c>
-      <c r="I8" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E9" s="5">
-        <v>0.67</v>
-      </c>
-      <c r="F9" s="3">
-        <v>3</v>
-      </c>
-      <c r="G9" s="3">
-        <f t="shared" ref="G9" si="2">F9*4</f>
-        <v>12</v>
-      </c>
-      <c r="H9" s="5">
-        <f t="shared" ref="H9" si="3">E9*G9</f>
-        <v>8.0400000000000009</v>
-      </c>
-      <c r="I9" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="E10" s="1"/>
-      <c r="G10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H10" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="E11" s="1"/>
-      <c r="G11">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H11" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="E12" s="1"/>
-      <c r="G12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H12" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C12" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="5">
+        <v>2.38</v>
+      </c>
+      <c r="F12" s="3">
+        <v>1</v>
+      </c>
+      <c r="G12" s="3">
+        <f t="shared" ref="G12" si="6">F12*4</f>
+        <v>4</v>
+      </c>
+      <c r="H12" s="5">
+        <f t="shared" ref="H12" si="7">E12*G12</f>
+        <v>9.52</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="O12" s="8"/>
+      <c r="P12" s="8"/>
+      <c r="Q12" s="8"/>
+      <c r="R12" s="8"/>
+      <c r="S12" s="8"/>
+      <c r="T12" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="U12" s="8">
+        <v>6.99</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="E13" s="1"/>
       <c r="G13">
         <f t="shared" si="0"/>
@@ -794,8 +1136,15 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="O13" s="8"/>
+      <c r="P13" s="8"/>
+      <c r="Q13" s="8"/>
+      <c r="R13" s="8"/>
+      <c r="S13" s="8"/>
+      <c r="T13" s="8"/>
+      <c r="U13" s="8"/>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="E14" s="1"/>
       <c r="G14">
         <f t="shared" si="0"/>
@@ -805,8 +1154,15 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="O14" s="8"/>
+      <c r="P14" s="8"/>
+      <c r="Q14" s="8"/>
+      <c r="R14" s="8"/>
+      <c r="S14" s="8"/>
+      <c r="T14" s="8"/>
+      <c r="U14" s="8"/>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="E15" s="1"/>
       <c r="G15">
         <f t="shared" si="0"/>
@@ -816,8 +1172,15 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="O15" s="8"/>
+      <c r="P15" s="8"/>
+      <c r="Q15" s="8"/>
+      <c r="R15" s="8"/>
+      <c r="S15" s="8"/>
+      <c r="T15" s="8"/>
+      <c r="U15" s="8"/>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="E16" s="1"/>
       <c r="G16">
         <f t="shared" si="0"/>
@@ -826,6 +1189,16 @@
       <c r="H16" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
+      </c>
+      <c r="O16" s="8"/>
+      <c r="P16" s="8"/>
+      <c r="Q16" s="8"/>
+      <c r="R16" s="8"/>
+      <c r="S16" s="8"/>
+      <c r="T16" s="8"/>
+      <c r="U16" s="9">
+        <f>SUM(U4:U12)</f>
+        <v>20.808</v>
       </c>
     </row>
     <row r="17" spans="5:8" x14ac:dyDescent="0.25">
@@ -841,6 +1214,14 @@
     </row>
     <row r="18" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E18" s="1"/>
+      <c r="G18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H18" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="19" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E19" s="1"/>
@@ -1075,6 +1456,9 @@
     </row>
     <row r="96" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E96" s="1"/>
+    </row>
+    <row r="97" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E97" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>